<commit_message>
Rebuild RoadCatalog and fix some bug in C_POI.xlsx
</commit_message>
<xml_diff>
--- a/conf/excel/C_SubwayST.xlsx
+++ b/conf/excel/C_SubwayST.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\长期文件\学习资料\综合学习资料\tencent\配置文件相关\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\学习资料\综合学习资料\tencent\配置文件相关\newCA-config-final\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE3F3219-2F6C-48A3-8D77-4C8BCBE857D3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34A00EB9-9752-44BF-8C05-882A9D3DDD35}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1320" yWindow="1125" windowWidth="23580" windowHeight="10035" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="C_SubwayST.conf" sheetId="1" r:id="rId1"/>
@@ -124,27 +124,18 @@
     <t>注释说明</t>
   </si>
   <si>
-    <t>status=1;point_type=8</t>
-  </si>
-  <si>
     <t>catalog=010A0303</t>
   </si>
   <si>
     <t>换乘地铁站</t>
   </si>
   <si>
-    <t>status=1;line_id=1000000000056042</t>
-  </si>
-  <si>
     <t>catalog=010A030101</t>
   </si>
   <si>
     <t>普通地铁站深圳市龙华线</t>
   </si>
   <si>
-    <t>status=1;line_id=1000000000056043</t>
-  </si>
-  <si>
     <t>status=1</t>
   </si>
   <si>
@@ -167,6 +158,18 @@
   </si>
   <si>
     <t>#status!="1"&amp;&amp;line_id=&lt;(C_SubwayLine, status!=1)-&gt;line_id</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>status=1;point_type="8"</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>status=1;line_id=“1000000000056042”</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>status=1;line_id=“1000000000056043”</t>
     <phoneticPr fontId="5" type="noConversion"/>
   </si>
 </sst>
@@ -174,7 +177,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -217,6 +220,14 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="等线"/>
+      <family val="3"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -253,7 +264,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -273,6 +284,9 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -552,7 +566,7 @@
   <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -589,66 +603,66 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="5" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="C5" s="4" t="s">
         <v>6</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>10</v>
-      </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A7" s="4" t="s">
-        <v>11</v>
+      <c r="A7" s="8" t="s">
+        <v>19</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
     <row r="9" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A9" s="4"/>
       <c r="B9" s="4" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>